<commit_message>
ITSADSSD-15851 Dev: Exchange Processes GetAppCredentials exports plain text for exchange activities GetTransactionData set to exchange InitExchange verifies account and folder access
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RPATask1-ChartStringProformaDetail\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\RPATask1-ChartStringProformaDetail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Exchange" sheetId="5" r:id="rId4"/>
+    <sheet name="Exceptions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -174,13 +176,85 @@
   </si>
   <si>
     <t>DEV</t>
+  </si>
+  <si>
+    <t>Proforma-DEV-Exchange</t>
+  </si>
+  <si>
+    <t>ExchangeCreds</t>
+  </si>
+  <si>
+    <t>s.janetzki@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Credential</t>
+  </si>
+  <si>
+    <t>ExchangeInbox</t>
+  </si>
+  <si>
+    <t>ExchangeOutbox</t>
+  </si>
+  <si>
+    <t>ExchangeExceptions</t>
+  </si>
+  <si>
+    <t>ExchangeMonitors</t>
+  </si>
+  <si>
+    <t>ExchangeSupervisors</t>
+  </si>
+  <si>
+    <t>Development\Proforma\Robot Out</t>
+  </si>
+  <si>
+    <t>Development\Proforma\Robot Error</t>
+  </si>
+  <si>
+    <t>Development\Proforma\Robot In</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>The configuration file {0} does not exist</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>The account for {0} could not be reached</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>LogMessage_ExchangeAccount</t>
+  </si>
+  <si>
+    <t>LogMessage_ExchangeFolder</t>
+  </si>
+  <si>
+    <t>The folder {0} was not found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,6 +265,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -198,16 +273,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF54646C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9FAFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,16 +316,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1583,7 +1702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1767,48 +1888,18 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2793,16 +2884,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="65.42578125" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="27" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2810,9 +2905,11 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2835,22 +2932,30 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:27" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3838,4 +3943,189 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
+    <col min="4" max="4" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ITSADSSD-15854 Dev: UniFi Processes 0. ConfigDev 1: LoginUniFi 2: NavToMainMenuItem 3: LogoutUniFi 4. Search RMNumber 5. Update RM Proposal
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Exchange" sheetId="5" r:id="rId4"/>
     <sheet name="Exceptions" sheetId="6" r:id="rId5"/>
+    <sheet name="Messages" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -181,9 +182,6 @@
     <t>Proforma-DEV-Exchange</t>
   </si>
   <si>
-    <t>ExchangeCreds</t>
-  </si>
-  <si>
     <t>s.janetzki@uq.edu.au</t>
   </si>
   <si>
@@ -226,12 +224,6 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>The account for {0} could not be reached</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -241,20 +233,134 @@
     <t>0.3</t>
   </si>
   <si>
-    <t>LogMessage_ExchangeAccount</t>
-  </si>
-  <si>
-    <t>LogMessage_ExchangeFolder</t>
-  </si>
-  <si>
-    <t>The folder {0} was not found</t>
+    <t>The folder {0} was not found under account {1}.</t>
+  </si>
+  <si>
+    <t>Proforma-DEV-UniFi</t>
+  </si>
+  <si>
+    <t>UniFi_URL</t>
+  </si>
+  <si>
+    <t>https://fs92rept.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>CredentialsUniFi</t>
+  </si>
+  <si>
+    <t>CredentialsExchange</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>I couldn't find any emails in my in tray!</t>
+  </si>
+  <si>
+    <t>I couldn't find any data in email!</t>
+  </si>
+  <si>
+    <t>I couldn't find correct format in email!</t>
+  </si>
+  <si>
+    <t>I couldn't find correct data in email!</t>
+  </si>
+  <si>
+    <t>I couldn't get into UniFi!</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>I couldn't get into UniFi! Need to reset password</t>
+  </si>
+  <si>
+    <t>I couldn't get find 'Maintain Staged Proposals' field in UniFi!</t>
+  </si>
+  <si>
+    <t>I couldn't find 'RM Number' in subject line in email!</t>
+  </si>
+  <si>
+    <t>I couldn't move Proforma email to Shared drive!</t>
+  </si>
+  <si>
+    <t>I couldn't match school code to accountant name UniFi!</t>
+  </si>
+  <si>
+    <t>I found blank data fields in UniFi!</t>
+  </si>
+  <si>
+    <t>I found data errors in UniFi!</t>
+  </si>
+  <si>
+    <t>I found a duplicate submission in UniFi!</t>
+  </si>
+  <si>
+    <t>I found invalid data in Proforma table in UniFi!</t>
+  </si>
+  <si>
+    <t>I found multiple 'RM Number's' in UniFi!</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>5.11</t>
+  </si>
+  <si>
+    <t>LogException_LoginUniFi</t>
+  </si>
+  <si>
+    <t>LogException_InitExchange</t>
+  </si>
+  <si>
+    <t>Grants\Proposals\Maintain Staged Proposals</t>
+  </si>
+  <si>
+    <t>Path from main menu to Proforma entry</t>
+  </si>
+  <si>
+    <t>NavToMSP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,12 +380,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF54646C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -294,21 +394,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9FAFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -316,31 +410,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFE0E0E0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -625,7 +711,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -700,7 +786,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1694,6 +1787,9 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1702,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1877,26 +1973,16 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-    </row>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2886,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2905,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2934,15 +3020,22 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3950,7 +4043,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,71 +4054,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -4034,7 +4128,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="63.5703125" customWidth="1"/>
     <col min="4" max="4" width="89" customWidth="1"/>
   </cols>
@@ -4043,8 +4137,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>63</v>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4054,19 +4148,19 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>69</v>
+      <c r="B3" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -4079,8 +4173,8 @@
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>70</v>
+      <c r="B4" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -4093,8 +4187,8 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>71</v>
+      <c r="B5" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -4104,25 +4198,233 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>66</v>
+      <c r="A7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B10:B14" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
+    <col min="4" max="4" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extra development of test files for UniFi search. Enhanced log messages for all current progress.
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,15 @@
     <sheet name="Exceptions" sheetId="6" r:id="rId5"/>
     <sheet name="Messages" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Exceptions!$A$1:$D$18</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -122,9 +125,6 @@
     <t>LogMessage_GetTransactionDataError</t>
   </si>
   <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
     <t>Static part of logging message. Error retrieving Transaction Data.</t>
   </si>
   <si>
@@ -140,18 +140,12 @@
     <t>LogMessage_BusinessRuleException</t>
   </si>
   <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
     <t>Static part of logging message. Processed Transaction failed with business exception</t>
   </si>
   <si>
     <t>LogMessage_ApplicationException</t>
   </si>
   <si>
-    <t>System exception.</t>
-  </si>
-  <si>
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
@@ -218,12 +212,6 @@
     <t>0.0</t>
   </si>
   <si>
-    <t>The configuration file {0} does not exist</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -233,9 +221,6 @@
     <t>0.3</t>
   </si>
   <si>
-    <t>The folder {0} was not found under account {1}.</t>
-  </si>
-  <si>
     <t>Proforma-DEV-UniFi</t>
   </si>
   <si>
@@ -251,109 +236,190 @@
     <t>CredentialsExchange</t>
   </si>
   <si>
-    <t>4.1</t>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Grants\Proposals\Maintain Staged Proposals</t>
+  </si>
+  <si>
+    <t>Path from main menu to Proforma entry</t>
+  </si>
+  <si>
+    <t>Config Error</t>
+  </si>
+  <si>
+    <t>System Error</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>I couldn't find any emails in my in tray!</t>
-  </si>
-  <si>
-    <t>I couldn't find any data in email!</t>
-  </si>
-  <si>
-    <t>I couldn't find correct format in email!</t>
-  </si>
-  <si>
-    <t>I couldn't find correct data in email!</t>
-  </si>
-  <si>
-    <t>I couldn't get into UniFi!</t>
-  </si>
-  <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>4.4</t>
-  </si>
-  <si>
-    <t>5.6</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>I couldn't get into UniFi! Need to reset password</t>
-  </si>
-  <si>
-    <t>I couldn't get find 'Maintain Staged Proposals' field in UniFi!</t>
-  </si>
-  <si>
-    <t>I couldn't find 'RM Number' in subject line in email!</t>
-  </si>
-  <si>
-    <t>I couldn't move Proforma email to Shared drive!</t>
-  </si>
-  <si>
-    <t>I couldn't match school code to accountant name UniFi!</t>
-  </si>
-  <si>
-    <t>I found blank data fields in UniFi!</t>
-  </si>
-  <si>
-    <t>I found data errors in UniFi!</t>
-  </si>
-  <si>
-    <t>I found a duplicate submission in UniFi!</t>
-  </si>
-  <si>
-    <t>I found invalid data in Proforma table in UniFi!</t>
-  </si>
-  <si>
-    <t>I found multiple 'RM Number's' in UniFi!</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>5.4</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>5.7</t>
-  </si>
-  <si>
-    <t>5.8</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>5.10</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
-    <t>LogException_LoginUniFi</t>
-  </si>
-  <si>
-    <t>LogException_InitExchange</t>
-  </si>
-  <si>
-    <t>Grants\Proposals\Maintain Staged Proposals</t>
-  </si>
-  <si>
-    <t>Path from main menu to Proforma entry</t>
-  </si>
-  <si>
-    <t>NavToMSP</t>
+    <t>Invalid Proforma Data</t>
+  </si>
+  <si>
+    <t>The accountant lookup file was not found at {0}</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2-6</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Accountant Not Found</t>
+  </si>
+  <si>
+    <t>9.1-5</t>
+  </si>
+  <si>
+    <t>I couldn't match {0} to an accountant name</t>
+  </si>
+  <si>
+    <t>I couldn't find my configuration file at {0}</t>
+  </si>
+  <si>
+    <t>SystemError_InitExchange</t>
+  </si>
+  <si>
+    <t>SystemError_AccountantFile</t>
+  </si>
+  <si>
+    <t>SystemError_LoginUniFi</t>
+  </si>
+  <si>
+    <t>SystemError_NavigateUniFi</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateProforma</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateRMNum</t>
+  </si>
+  <si>
+    <t>RuleException_SearchRMNum</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>Exchange Error</t>
+  </si>
+  <si>
+    <t>Network Error</t>
+  </si>
+  <si>
+    <t>9.7-10</t>
+  </si>
+  <si>
+    <t>Invalid RM Number</t>
+  </si>
+  <si>
+    <t>No Search Results</t>
+  </si>
+  <si>
+    <t>I couldn't match {0} as the RM number in the email</t>
+  </si>
+  <si>
+    <t>No Updated Entries</t>
+  </si>
+  <si>
+    <t>SystemError_ProformaEntry</t>
+  </si>
+  <si>
+    <t>10.2-11.3</t>
+  </si>
+  <si>
+    <t>12.1-9</t>
+  </si>
+  <si>
+    <t>I searched for {0} and found no results</t>
+  </si>
+  <si>
+    <t>I couldn't find any emails in {0}</t>
+  </si>
+  <si>
+    <t>I couldn't verify {0} as {1} in the Proforma table</t>
+  </si>
+  <si>
+    <t>RuleException_NoEmails</t>
+  </si>
+  <si>
+    <t>No Emails Found</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>I couldn't create the folder at {0}</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>SystemError_CreateFolder</t>
+  </si>
+  <si>
+    <t>SystemError_SaveEmail</t>
+  </si>
+  <si>
+    <t>I couldn't save the email to {0}</t>
+  </si>
+  <si>
+    <t>UniFiPath_MaintainStagedProposals</t>
+  </si>
+  <si>
+    <t>I couldn't login as {0} to UniFi at {1}</t>
+  </si>
+  <si>
+    <t>SystemError_CheckExchange</t>
+  </si>
+  <si>
+    <t>I couldn’t find {0} when checking {1}</t>
+  </si>
+  <si>
+    <t>I couldn't check my emails as {0}</t>
+  </si>
+  <si>
+    <t>UniFi Login Error</t>
+  </si>
+  <si>
+    <t>UniFi Navigation Error</t>
+  </si>
+  <si>
+    <t>UniFi Updating Error</t>
+  </si>
+  <si>
+    <t>RuleException_SearchAccountant</t>
+  </si>
+  <si>
+    <t>Rule Exception</t>
+  </si>
+  <si>
+    <t>I got lost while navigating to {0}</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledUniFi</t>
+  </si>
+  <si>
+    <t>9.1-12.9</t>
+  </si>
+  <si>
+    <t>UniFi Unknown Error</t>
+  </si>
+  <si>
+    <t>I wasn't able to update {0} as the rows were: {1}</t>
+  </si>
+  <si>
+    <t>RuleException_UpdateProforma</t>
+  </si>
+  <si>
+    <t>I couldn't update row {0} due to: {1}</t>
   </si>
 </sst>
 </file>
@@ -415,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -427,6 +493,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,7 +778,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -758,40 +825,40 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1798,7 +1865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1972,14 +2039,14 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>109</v>
+      <c r="A19" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2973,7 +3040,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2991,7 +3058,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3022,18 +3089,18 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>68</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4043,7 +4110,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,42 +4133,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4119,10 +4186,351 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
+    <col min="4" max="4" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="7"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D15">
+    <sortState ref="A2:D15">
+      <sortCondition ref="A1:A15"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4138,265 +4546,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B10:B14" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" customWidth="1"/>
-    <col min="4" max="4" width="89" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4418,13 +4568,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ITSADSSD-16014 - finished end to end test scenario Removed the robot retry activities - managed through orch
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="Messages" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Exceptions!$A$1:$D$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Exceptions!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
-  </si>
-  <si>
     <t>TimeoutShort</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>DEV-none</t>
-  </si>
-  <si>
     <t>Chart String Proforma Detail</t>
   </si>
   <si>
@@ -420,6 +411,39 @@
   </si>
   <si>
     <t>I couldn't update row {0} due to: {1}</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledExchange</t>
+  </si>
+  <si>
+    <t>7.1-6</t>
+  </si>
+  <si>
+    <t>Unknown Scrape Error</t>
+  </si>
+  <si>
+    <t>I couldn't scrape proforma data from the email {0}</t>
+  </si>
+  <si>
+    <t>DEV-ChartStringProforma</t>
+  </si>
+  <si>
+    <t>LogMessage_SkippedProforma</t>
+  </si>
+  <si>
+    <t>LogMessage_UpdatedProforma</t>
+  </si>
+  <si>
+    <t>Row {0} skipped, {1}</t>
+  </si>
+  <si>
+    <t>Row {0} updated, {1}</t>
+  </si>
+  <si>
+    <t>Trimm_StorageFolder</t>
+  </si>
+  <si>
+    <t>Q:\ITS\ITS-Dropbox\uqsjanet\Dev\Proforma\{0}\</t>
   </si>
 </sst>
 </file>
@@ -778,7 +802,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -825,43 +849,50 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1858,15 +1889,16 @@
     <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1917,138 +1949,128 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>30000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>5000</v>
+        <v>120000</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>30000</v>
-      </c>
-      <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>120000</v>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
         <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>15000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>15000</v>
-      </c>
-      <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>60000</v>
+        <v>0.6</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16">
-        <v>0.8</v>
-      </c>
-      <c r="C16" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17">
-        <v>0.9</v>
+      <c r="A17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3028,8 +3050,6 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3040,7 +3060,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3058,7 +3078,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3089,18 +3109,18 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4109,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4133,42 +4153,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4186,10 +4206,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4205,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4216,268 +4236,278 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>82</v>
+        <v>128</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>115</v>
+        <v>130</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>126</v>
+        <v>109</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="D24" s="7"/>
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -4488,34 +4518,38 @@
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="D27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
+      <c r="B28" s="10"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="9"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
+      <c r="B30" s="10"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
+      <c r="B31" s="9"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
+      <c r="B32" s="10"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D15">
+  <autoFilter ref="A1:D16">
     <sortState ref="A2:D15">
       <sortCondition ref="A1:A15"/>
     </sortState>
@@ -4527,10 +4561,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,7 +4580,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4557,24 +4591,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing of email sending capabilities and network file access impersonation
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,25 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Exchange" sheetId="5" r:id="rId4"/>
-    <sheet name="Exceptions" sheetId="6" r:id="rId5"/>
-    <sheet name="Messages" sheetId="7" r:id="rId6"/>
+    <sheet name="Messages" sheetId="7" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Exceptions!$A$1:$D$19</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -131,12 +127,6 @@
     <t>Static part of logging message. Processed Transaction succesful</t>
   </si>
   <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception</t>
-  </si>
-  <si>
     <t>LogMessage_ApplicationException</t>
   </si>
   <si>
@@ -206,9 +196,6 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>0.3</t>
   </si>
   <si>
@@ -387,9 +374,6 @@
   </si>
   <si>
     <t>RuleException_SearchAccountant</t>
-  </si>
-  <si>
-    <t>Rule Exception</t>
   </si>
   <si>
     <t>I got lost while navigating to {0}</t>
@@ -505,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -515,7 +499,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -849,48 +832,48 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2060,13 +2043,13 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3078,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3109,18 +3092,18 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4129,7 +4112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4153,42 +4136,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4206,365 +4189,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" customWidth="1"/>
-    <col min="4" max="4" width="89" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="7"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D16">
-    <sortState ref="A2:D15">
-      <sortCondition ref="A1:A15"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4580,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4590,43 +4218,304 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C25" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="2" t="s">
-        <v>136</v>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Share drive mapping changes Email report progress
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t>Q:\ITS\ITS-Dropbox\uqsjanet\Dev\Proforma\{0}\</t>
+  </si>
+  <si>
+    <t>Proforma-DEV-Network</t>
+  </si>
+  <si>
+    <t>CredentialsNetwork</t>
+  </si>
+  <si>
+    <t>Q: \\nas02.storage.uq.edu.au\CA</t>
+  </si>
+  <si>
+    <t>NetworkShareDrive</t>
   </si>
 </sst>
 </file>
@@ -785,7 +797,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -876,7 +888,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3042,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3106,7 +3125,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4191,7 +4217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ITSADSSD-16016 Finished job summary email generation
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,21 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
-    <sheet name="Exchange" sheetId="5" r:id="rId4"/>
-    <sheet name="Messages" sheetId="7" r:id="rId5"/>
+    <sheet name="Messages" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -235,9 +234,6 @@
     <t>Invalid Proforma Data</t>
   </si>
   <si>
-    <t>The accountant lookup file was not found at {0}</t>
-  </si>
-  <si>
     <t>7.1</t>
   </si>
   <si>
@@ -322,9 +318,6 @@
     <t>I couldn't find any emails in {0}</t>
   </si>
   <si>
-    <t>I couldn't verify {0} as {1} in the Proforma table</t>
-  </si>
-  <si>
     <t>RuleException_NoEmails</t>
   </si>
   <si>
@@ -352,18 +345,9 @@
     <t>UniFiPath_MaintainStagedProposals</t>
   </si>
   <si>
-    <t>I couldn't login as {0} to UniFi at {1}</t>
-  </si>
-  <si>
     <t>SystemError_CheckExchange</t>
   </si>
   <si>
-    <t>I couldn’t find {0} when checking {1}</t>
-  </si>
-  <si>
-    <t>I couldn't check my emails as {0}</t>
-  </si>
-  <si>
     <t>UniFi Login Error</t>
   </si>
   <si>
@@ -440,13 +424,82 @@
   </si>
   <si>
     <t>NetworkShareDrive</t>
+  </si>
+  <si>
+    <t>Data\EmailLogo.png</t>
+  </si>
+  <si>
+    <t>Minion logo for email signature</t>
+  </si>
+  <si>
+    <t>HTML file containing parts to build end of job report</t>
+  </si>
+  <si>
+    <t>HTML file containing parts to build the weekly summary</t>
+  </si>
+  <si>
+    <t>Email_Logo</t>
+  </si>
+  <si>
+    <t>Data\JobTemplate.html</t>
+  </si>
+  <si>
+    <t>Data\WeeklyTemplate.html</t>
+  </si>
+  <si>
+    <t>Email_Weekly</t>
+  </si>
+  <si>
+    <t>Email_Job</t>
+  </si>
+  <si>
+    <t>Accountant Lookup.xlsx</t>
+  </si>
+  <si>
+    <t>Accountant username lookup file</t>
+  </si>
+  <si>
+    <t>Nvision</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook</t>
+  </si>
+  <si>
+    <t>Accountant_LookupSheet</t>
+  </si>
+  <si>
+    <t>{0} has validation issues with {1}</t>
+  </si>
+  <si>
+    <t>Problems loading {0} for Acc lookup: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>Problems with {0}'s mail: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>Problems checking {0} as {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>ExchangeExitErrors</t>
+  </si>
+  <si>
+    <t>ExchangeExitSuccess</t>
+  </si>
+  <si>
+    <t>Proforma documents processed successfully</t>
+  </si>
+  <si>
+    <t>Errors processing proforma documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -461,13 +514,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -499,14 +545,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -797,7 +842,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -844,31 +889,20 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -876,51 +910,137 @@
       <c r="A5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1889,9 +2009,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1899,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1945,147 +2066,148 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>5000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>30000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>120000</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>1000</v>
+        <v>15000</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>60000</v>
-      </c>
-      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>0.9</v>
-      </c>
-      <c r="C15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3061,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3113,7 +3235,7 @@
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3121,16 +3243,16 @@
       <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4136,95 +4258,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="63.5703125" customWidth="1"/>
     <col min="4" max="4" width="89" customWidth="1"/>
   </cols>
@@ -4233,7 +4276,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4244,243 +4287,243 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>77</v>
+      <c r="D4" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>86</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>95</v>
+        <v>117</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>103</v>
+        <v>87</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="10" t="s">
         <v>104</v>
       </c>
+      <c r="B19" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" s="8"/>
+        <v>115</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C22" t="s">
@@ -4494,7 +4537,7 @@
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C23" t="s">
@@ -4528,20 +4571,20 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>129</v>
-      </c>
-      <c r="B26" s="10"/>
+        <v>124</v>
+      </c>
+      <c r="B26" s="9"/>
       <c r="C26" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="10"/>
+        <v>125</v>
+      </c>
+      <c r="B27" s="9"/>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated signature to match UQ template Expanding testing cases
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
     <t>TimeoutShort</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>Chart String Proforma Detail</t>
-  </si>
-  <si>
     <t>ProcessMode</t>
   </si>
   <si>
@@ -414,12 +408,6 @@
     <t>Q:\ITS\ITS-Dropbox\uqsjanet\Dev\Proforma\{0}\</t>
   </si>
   <si>
-    <t>Proforma-DEV-Network</t>
-  </si>
-  <si>
-    <t>CredentialsNetwork</t>
-  </si>
-  <si>
     <t>Q: \\nas02.storage.uq.edu.au\CA</t>
   </si>
   <si>
@@ -493,6 +481,36 @@
   </si>
   <si>
     <t>Errors processing proforma documents</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Comments (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>SSO_rpa00001</t>
+  </si>
+  <si>
+    <t>SSO Credentials</t>
+  </si>
+  <si>
+    <t>CredentialsFileShare</t>
+  </si>
+  <si>
+    <t>Proforma-DEV-FileShare</t>
+  </si>
+  <si>
+    <t>Email_Banner</t>
+  </si>
+  <si>
+    <t>Data\UQBanner.png</t>
+  </si>
+  <si>
+    <t>UQ banner for email signature</t>
+  </si>
+  <si>
+    <t>Minion</t>
   </si>
 </sst>
 </file>
@@ -547,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -558,6 +576,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -841,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -861,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -889,148 +908,159 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>137</v>
+      </c>
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2020,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2068,139 +2098,139 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>5000</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>30000</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>120000</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>1000</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>15000</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>60000</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>0.6</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>0.8</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>0.9</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3184,7 +3214,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3202,10 +3232,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3233,29 +3263,36 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4258,10 +4295,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4269,15 +4306,16 @@
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="63.5703125" customWidth="1"/>
-    <col min="4" max="4" width="89" customWidth="1"/>
+    <col min="4" max="4" width="60.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4285,309 +4323,313 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
         <v>29</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
         <v>34</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Friday commit, pulling config references out of job report to ease distribution of workflow without the re framework being required, uat and prod email access tested, still working on uat and prod file access
</commit_message>
<xml_diff>
--- a/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
+++ b/Processes/RPATask1-ChartStringProformaDetail/Data/ConfigDev.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -511,6 +511,39 @@
   </si>
   <si>
     <t>Minion</t>
+  </si>
+  <si>
+    <t>Testing_ReportWorkbook</t>
+  </si>
+  <si>
+    <t>Test_Framework\TestReportSummary.xlsx</t>
+  </si>
+  <si>
+    <t>Location of the test file to output results of job report generation</t>
+  </si>
+  <si>
+    <t>Testing_ReportSheet</t>
+  </si>
+  <si>
+    <t>ReportResults</t>
+  </si>
+  <si>
+    <t>Worksheet to output results of test job report generation</t>
+  </si>
+  <si>
+    <t>Testing_SummaryWorkbook</t>
+  </si>
+  <si>
+    <t>Testing_SummarySheet</t>
+  </si>
+  <si>
+    <t>SummaryResults</t>
+  </si>
+  <si>
+    <t>Worksheet to output results of test weekly summary generation</t>
+  </si>
+  <si>
+    <t>Location of the test file to output results of weekly summary generation</t>
   </si>
 </sst>
 </file>
@@ -858,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -979,94 +1012,134 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>130</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>160</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C25" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>135</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B27" t="s">
         <v>136</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C27" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2036,10 +2109,14 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>